<commit_message>
Some processing, made slight modifications
</commit_message>
<xml_diff>
--- a/GDP.xlsx
+++ b/GDP.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t xml:space="preserve">Series Name</t>
   </si>
@@ -38,9 +38,69 @@
     <t xml:space="preserve">1990 [YR1990]</t>
   </si>
   <si>
+    <t xml:space="preserve">1991 [YR1991]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1992 [YR1992]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1993 [YR1993]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1994 [YR1994]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1995 [YR1995]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1996 [YR1996]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1997 [YR1997]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1998 [YR1998]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1999 [YR1999]</t>
+  </si>
+  <si>
     <t xml:space="preserve">2000 [YR2000]</t>
   </si>
   <si>
+    <t xml:space="preserve">2001 [YR2001]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002 [YR2002]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003 [YR2003]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004 [YR2004]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2005 [YR2005]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2006 [YR2006]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2007 [YR2007]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008 [YR2008]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009 [YR2009]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010 [YR2010]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011 [YR2011]</t>
+  </si>
+  <si>
     <t xml:space="preserve">2012 [YR2012]</t>
   </si>
   <si>
@@ -65,28 +125,22 @@
     <t xml:space="preserve">2019 [YR2019]</t>
   </si>
   <si>
-    <t xml:space="preserve">2020 [YR2020]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 [YR2021]</t>
-  </si>
-  <si>
     <t xml:space="preserve">GDP per capita (current US$)</t>
   </si>
   <si>
     <t xml:space="preserve">NY.GDP.PCAP.CD</t>
   </si>
   <si>
+    <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBR</t>
+  </si>
+  <si>
     <t xml:space="preserve">India</t>
   </si>
   <si>
     <t xml:space="preserve">IND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBR</t>
   </si>
   <si>
     <t xml:space="preserve">Code</t>
@@ -217,8 +271,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -247,181 +305,345 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="7:8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM14" activeCellId="0" sqref="AM14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>19095.4669984608</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>19900.7266505069</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>20487.1707852878</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>18389.0195675099</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>19709.2380983653</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>23202.4615775949</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>24440.3281377791</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>26781.362168176</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>28297.8659970584</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>28786.9592756835</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>28290.9725024578</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>27886.7985907797</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>30079.6600435049</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>34479.3929332278</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>40390.7858294925</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>42131.6993992712</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>44536.6197203512</v>
+      </c>
+      <c r="V2" s="1" t="n">
+        <v>50435.37028921</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>47429.9363403009</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <v>38821.1795827116</v>
+      </c>
+      <c r="Y2" s="1" t="n">
+        <v>39693.1938701237</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <v>42150.6981408821</v>
+      </c>
+      <c r="AA2" s="1" t="n">
+        <v>42485.5860695397</v>
+      </c>
+      <c r="AB2" s="1" t="n">
+        <v>43449.0917173139</v>
+      </c>
+      <c r="AC2" s="1" t="n">
+        <v>47447.5889322667</v>
+      </c>
+      <c r="AD2" s="1" t="n">
+        <v>45071.0743234873</v>
+      </c>
+      <c r="AE2" s="1" t="n">
+        <v>41146.0773555246</v>
+      </c>
+      <c r="AF2" s="1" t="n">
+        <v>40621.334478632</v>
+      </c>
+      <c r="AG2" s="1" t="n">
+        <v>43306.3083049317</v>
+      </c>
+      <c r="AH2" s="1" t="n">
+        <v>42747.080460496</v>
+      </c>
+      <c r="AI2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>368.749759408129</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F3" s="1" t="n">
+        <v>303.850437957407</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>317.559135479384</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>301.501194948852</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>346.227393126042</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>373.628280320062</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>399.577503521552</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>414.898869576673</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>412.509511039641</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>440.961454614021</v>
+      </c>
+      <c r="O3" s="1" t="n">
         <v>442.034778917695</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="P3" s="1" t="n">
+        <v>449.911124933268</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>468.844428305181</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>543.843798893952</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>624.105094371897</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>710.509344850714</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>802.01374204738</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>1022.73162874643</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>993.503772474691</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>1096.63498033497</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>1350.63432207085</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>1449.60178853415</v>
+      </c>
+      <c r="AA3" s="1" t="n">
         <v>1434.01819806113</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="AB3" s="1" t="n">
         <v>1438.05748041006</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="AC3" s="1" t="n">
         <v>1559.86451848257</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="AD3" s="1" t="n">
         <v>1590.17391842781</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="AE3" s="1" t="n">
         <v>1714.28035526737</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="AF3" s="1" t="n">
         <v>1957.968841235</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="AG3" s="1" t="n">
         <v>1974.37778792366</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="AH3" s="1" t="n">
         <v>2047.23270433512</v>
       </c>
-      <c r="O2" s="0" t="n">
-        <v>1910.42147282449</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <v>2256.59040870506</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>19095.4669984608</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>28290.9725024578</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>42485.5860695397</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>43449.0917173139</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>47447.5889322667</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>45071.0743234873</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>41146.0773555246</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>40621.334478632</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>43306.3083049317</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>42747.080460496</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>40318.5575660493</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>46510.2827819127</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="AI3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -441,77 +663,77 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="7:8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="0" width="50.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="1" width="50.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>31</v>
+      <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>39</v>
+      <c r="D2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>